<commit_message>
Adding title and description tags
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1795D834-BFE9-8D4F-8ADA-D107EFBEA223}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DD68F5-5E7A-664C-88A0-09C4D2AE9C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>accessibility</t>
   </si>
@@ -216,20 +216,29 @@
     <t>x-compile-to-js</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Guide</t>
+  </si>
+  <si>
+    <t>Web Browser, Website, and Web Application Performance</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Generated Title Tag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -244,6 +253,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -276,9 +296,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -594,327 +616,757 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051CB134-E970-F24C-8599-A156C71AD5D0}">
-  <dimension ref="B1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="71.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" t="str">
+        <f>"&lt;title&gt;Learning "&amp;C2&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
+        <v>&lt;title&gt;Learning Accessibility Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E61" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
+        <v>&lt;title&gt;Learning Web Browser, Website, and Web Application Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3" t="s">
         <v>59</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use emojis for read/watch/paid, updated header info, remove unused ci guide
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DD68F5-5E7A-664C-88A0-09C4D2AE9C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EEA913-8C48-F34E-83C2-12A6741C734F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>accessibility</t>
   </si>
@@ -42,9 +42,6 @@
     <t>browser-webpage-performance</t>
   </si>
   <si>
-    <t>buildspec.yml</t>
-  </si>
-  <si>
     <t>ci</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>Guide</t>
   </si>
   <si>
-    <t>Web Browser, Website, and Web Application Performance</t>
-  </si>
-  <si>
     <t>Accessibility</t>
   </si>
   <si>
@@ -232,6 +226,9 @@
   </si>
   <si>
     <t>Generated Title Tag</t>
+  </si>
+  <si>
+    <t>Browser, Website, and Web Application Performance</t>
   </si>
 </sst>
 </file>
@@ -616,33 +613,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051CB134-E970-F24C-8599-A156C71AD5D0}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" customWidth="1"/>
-    <col min="4" max="4" width="58.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="3" max="3" width="52.5" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -651,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="str">
@@ -665,12 +662,12 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E61" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Web Browser, Website, and Web Application Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <f t="shared" ref="E3:E60" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
+        <v>&lt;title&gt;Learning Browser, Website, and Web Application Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1357,18 +1354,6 @@
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix the repo link
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EEA913-8C48-F34E-83C2-12A6741C734F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453ADC17-D1E4-3248-AE7C-A51A8F5562C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>accessibility</t>
   </si>
@@ -42,9 +42,6 @@
     <t>browser-webpage-performance</t>
   </si>
   <si>
-    <t>ci</t>
-  </si>
-  <si>
     <t>code-editors</t>
   </si>
   <si>
@@ -219,16 +216,40 @@
     <t>Guide</t>
   </si>
   <si>
-    <t>Accessibility</t>
-  </si>
-  <si>
     <t>Topic</t>
   </si>
   <si>
     <t>Generated Title Tag</t>
   </si>
   <si>
-    <t>Browser, Website, and Web Application Performance</t>
+    <t>Generated Meta Tag</t>
+  </si>
+  <si>
+    <t>Test description</t>
+  </si>
+  <si>
+    <t>Learn Accessibility</t>
+  </si>
+  <si>
+    <t>Learn Browser, Website, and Web App Performance</t>
+  </si>
+  <si>
+    <t>Learn Code Editors</t>
+  </si>
+  <si>
+    <t>Learn the Command Line Interface</t>
+  </si>
+  <si>
+    <t>Learn CSS Fonts &amp; Icons</t>
+  </si>
+  <si>
+    <t>Learn CSS Fundamentals</t>
+  </si>
+  <si>
+    <t>Learn CSS in JavaScript</t>
+  </si>
+  <si>
+    <t>Learn CSS Layout</t>
   </si>
 </sst>
 </file>
@@ -613,136 +634,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051CB134-E970-F24C-8599-A156C71AD5D0}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="3" max="3" width="52.5" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" customWidth="1"/>
     <col min="4" max="4" width="65.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="5" max="5" width="104.83203125" customWidth="1"/>
+    <col min="6" max="6" width="85.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="E2" t="str">
         <f>"&lt;title&gt;Learning "&amp;C2&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Accessibility Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn Accessibility Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"&lt;meta name='description' content=''"&amp;D2&amp;"'&gt;"</f>
+        <v>&lt;meta name='description' content=''Test description'&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E60" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Browser, Website, and Web Application Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <f t="shared" ref="E3:E59" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
+        <v>&lt;title&gt;Learning Learn Browser, Website, and Web App Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F59" si="1">"&lt;meta name='description' content=''"&amp;D3&amp;"'&gt;"</f>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn Code Editors Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn the Command Line Interface Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn CSS Fonts &amp; Icons Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn CSS Fundamentals Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn CSS in JavaScript Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>&lt;title&gt;Learning Learn CSS Layout Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -753,8 +824,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -765,8 +840,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -777,8 +856,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -789,8 +872,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>12</v>
@@ -801,8 +888,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>13</v>
@@ -813,8 +904,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>14</v>
@@ -825,8 +920,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>15</v>
@@ -837,8 +936,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>16</v>
@@ -849,8 +952,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>17</v>
@@ -861,8 +968,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>18</v>
@@ -873,8 +984,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>19</v>
@@ -885,8 +1000,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>20</v>
@@ -897,8 +1016,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>21</v>
@@ -909,8 +1032,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>22</v>
@@ -921,8 +1048,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>23</v>
@@ -933,8 +1064,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>24</v>
@@ -945,8 +1080,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>25</v>
@@ -957,8 +1096,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>26</v>
@@ -969,8 +1112,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
         <v>27</v>
@@ -981,8 +1128,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>28</v>
@@ -993,8 +1144,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
         <v>29</v>
@@ -1005,8 +1160,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
         <v>30</v>
@@ -1017,8 +1176,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>31</v>
@@ -1029,8 +1192,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>32</v>
@@ -1041,8 +1208,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
         <v>33</v>
@@ -1053,8 +1224,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>34</v>
@@ -1065,8 +1240,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
         <v>35</v>
@@ -1077,8 +1256,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>36</v>
@@ -1089,8 +1272,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
         <v>37</v>
@@ -1101,8 +1288,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>38</v>
@@ -1113,8 +1304,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
         <v>39</v>
@@ -1125,8 +1320,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>40</v>
@@ -1137,8 +1336,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
         <v>41</v>
@@ -1149,8 +1352,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>42</v>
@@ -1161,8 +1368,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>43</v>
@@ -1173,8 +1384,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
         <v>44</v>
@@ -1185,8 +1400,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>45</v>
@@ -1197,8 +1416,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>46</v>
@@ -1209,8 +1432,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>47</v>
@@ -1221,8 +1448,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
         <v>48</v>
@@ -1233,8 +1464,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
         <v>49</v>
@@ -1245,8 +1480,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
         <v>50</v>
@@ -1257,8 +1496,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
         <v>51</v>
@@ -1269,8 +1512,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="3" t="s">
         <v>52</v>
@@ -1281,8 +1528,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
         <v>53</v>
@@ -1293,8 +1544,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
         <v>54</v>
@@ -1305,8 +1560,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="3" t="s">
         <v>55</v>
@@ -1317,8 +1576,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3" t="s">
         <v>56</v>
@@ -1329,8 +1592,12 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="3" t="s">
         <v>57</v>
@@ -1341,17 +1608,9 @@
         <f t="shared" si="0"/>
         <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+      <c r="F59" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;meta name='description' content='''&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update URLs, File Structure, Meta Doc
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453ADC17-D1E4-3248-AE7C-A51A8F5562C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24561962-BC5B-F146-9BD4-3FC259607876}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>accessibility</t>
   </si>
@@ -69,9 +69,6 @@
     <t>css-tooling</t>
   </si>
   <si>
-    <t>css-transitions-transforms-&amp;-animations</t>
-  </si>
-  <si>
     <t>css-ui-toolkits</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>dom-bom-cssom</t>
   </si>
   <si>
-    <t>front-end-development-tech-overview</t>
-  </si>
-  <si>
     <t>getting-a-front-end-developer-job</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>http</t>
   </si>
   <si>
-    <t>index.html</t>
-  </si>
-  <si>
     <t>jam-stack</t>
   </si>
   <si>
@@ -177,21 +168,12 @@
     <t>seo</t>
   </si>
   <si>
-    <t>template</t>
-  </si>
-  <si>
     <t>testing</t>
   </si>
   <si>
-    <t>the-front-end-developer-profession</t>
-  </si>
-  <si>
     <t>the-web-platform</t>
   </si>
   <si>
-    <t>the-www-basic-mechanics</t>
-  </si>
-  <si>
     <t>ui-design-patterns</t>
   </si>
   <si>
@@ -225,31 +207,187 @@
     <t>Generated Meta Tag</t>
   </si>
   <si>
-    <t>Test description</t>
-  </si>
-  <si>
-    <t>Learn Accessibility</t>
-  </si>
-  <si>
-    <t>Learn Browser, Website, and Web App Performance</t>
-  </si>
-  <si>
-    <t>Learn Code Editors</t>
-  </si>
-  <si>
-    <t>Learn the Command Line Interface</t>
-  </si>
-  <si>
-    <t>Learn CSS Fonts &amp; Icons</t>
-  </si>
-  <si>
-    <t>Learn CSS Fundamentals</t>
-  </si>
-  <si>
-    <t>Learn CSS in JavaScript</t>
-  </si>
-  <si>
-    <t>Learn CSS Layout</t>
+    <t>Learning resources for eb accessibility means that everyone, including people with disabilities, can use your Websites.</t>
+  </si>
+  <si>
+    <t>Web Accessibility</t>
+  </si>
+  <si>
+    <t>Browser, Website, and Web App Performance</t>
+  </si>
+  <si>
+    <t>Code Editors</t>
+  </si>
+  <si>
+    <t>Command Line Interface</t>
+  </si>
+  <si>
+    <t>CSS Fonts &amp; Icons</t>
+  </si>
+  <si>
+    <t>CSS Fundamentals</t>
+  </si>
+  <si>
+    <t>CSS in JavaScript</t>
+  </si>
+  <si>
+    <t>CSS Layout</t>
+  </si>
+  <si>
+    <t>CSS Media Queries</t>
+  </si>
+  <si>
+    <t>CSS Best Practices</t>
+  </si>
+  <si>
+    <t>CSS Tooling</t>
+  </si>
+  <si>
+    <t>css-transitions-transforms-animations</t>
+  </si>
+  <si>
+    <t>front-end-developer-profession</t>
+  </si>
+  <si>
+    <t>www-basic-mechanics</t>
+  </si>
+  <si>
+    <t>CSS Transitions, Transforms, &amp; Animations</t>
+  </si>
+  <si>
+    <t>CSS UI Toolkits</t>
+  </si>
+  <si>
+    <t>Web Development Data APIs</t>
+  </si>
+  <si>
+    <t>Desktop Application Development with Web Technologies</t>
+  </si>
+  <si>
+    <t>DOM, BOM, &amp; CSSOM</t>
+  </si>
+  <si>
+    <t>The Front End Developer Profession</t>
+  </si>
+  <si>
+    <t>Front End Development Technology Overview</t>
+  </si>
+  <si>
+    <t>Getting a Front End Developer Job</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>HTML Email Development</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>JAM Stack</t>
+  </si>
+  <si>
+    <t>JavaScript Fundamentals</t>
+  </si>
+  <si>
+    <t>JavaScript Modules &amp; Scripts</t>
+  </si>
+  <si>
+    <t>JavaScript Regular Expressions</t>
+  </si>
+  <si>
+    <t>JavaScript Animation</t>
+  </si>
+  <si>
+    <t>JavaScript Application Frameworks/Libraries</t>
+  </si>
+  <si>
+    <t>JavaScript Asynchronous Programming</t>
+  </si>
+  <si>
+    <t>JavaScript Bundlers</t>
+  </si>
+  <si>
+    <t>JavaScript Compile to JS</t>
+  </si>
+  <si>
+    <t>JavaScript &amp; Computer Science</t>
+  </si>
+  <si>
+    <t>JavaScript Functional Programming (FP)</t>
+  </si>
+  <si>
+    <t>JavaScript Object-Oriented Programming (OOP)</t>
+  </si>
+  <si>
+    <t>JavaScript Performance</t>
+  </si>
+  <si>
+    <t>JavaScript Practices &amp; Tooling</t>
+  </si>
+  <si>
+    <t>JavaScript Runtime &amp; AST</t>
+  </si>
+  <si>
+    <t>JavaScript State Management</t>
+  </si>
+  <si>
+    <t>JavaScript UI Components and Widgets</t>
+  </si>
+  <si>
+    <t>JavaScript Web APIs</t>
+  </si>
+  <si>
+    <t>Native Mobile Applications</t>
+  </si>
+  <si>
+    <t>Node.js &amp; npm / Yarn</t>
+  </si>
+  <si>
+    <t>npm &amp; yarn Scripts</t>
+  </si>
+  <si>
+    <t>Progressive Web Apps (PWAs)</t>
+  </si>
+  <si>
+    <t>Responsive Web Design</t>
+  </si>
+  <si>
+    <t>Search Engine Optimization (SEO)</t>
+  </si>
+  <si>
+    <t>JavaScript Unit and End-to-End Testing</t>
+  </si>
+  <si>
+    <t>The Web Platform</t>
+  </si>
+  <si>
+    <t>UI Design / Patterns</t>
+  </si>
+  <si>
+    <t>Web Applications</t>
+  </si>
+  <si>
+    <t>Web Images</t>
+  </si>
+  <si>
+    <t>Web Security</t>
+  </si>
+  <si>
+    <t>Web Developer Tools</t>
+  </si>
+  <si>
+    <t>front-end-development-overview</t>
+  </si>
+  <si>
+    <t>Compile to JavaScript Languages</t>
+  </si>
+  <si>
+    <t>World Wide Web (WWW) Basic Mechanics</t>
   </si>
 </sst>
 </file>
@@ -636,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051CB134-E970-F24C-8599-A156C71AD5D0}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,19 +790,19 @@
     <row r="1" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -673,18 +811,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E2" t="str">
         <f>"&lt;title&gt;Learning "&amp;C2&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Learn Accessibility Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Web Accessibility Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F2" t="str">
         <f>"&lt;meta name='description' content=''"&amp;D2&amp;"'&gt;"</f>
-        <v>&lt;meta name='description' content=''Test description'&gt;</v>
+        <v>&lt;meta name='description' content=''Learning resources for eb accessibility means that everyone, including people with disabilities, can use your Websites.'&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -693,12 +831,12 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E59" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Learn Browser, Website, and Web App Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Browser, Website, and Web App Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F59" si="1">"&lt;meta name='description' content=''"&amp;D3&amp;"'&gt;"</f>
@@ -711,12 +849,12 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Learn Code Editors Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Code Editors Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -729,12 +867,12 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Learn the Command Line Interface Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Command Line Interface Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -747,12 +885,12 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Learn CSS Fonts &amp; Icons Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Fonts &amp; Icons Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -765,12 +903,12 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Learn CSS Fundamentals Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Fundamentals Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -783,12 +921,12 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Learn CSS in JavaScript Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS in JavaScript Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -801,12 +939,12 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Learn CSS Layout Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Layout Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -818,11 +956,13 @@
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Media Queries Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -834,11 +974,13 @@
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Best Practices Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -850,11 +992,13 @@
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Tooling Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -864,13 +1008,15 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS Transitions, Transforms, &amp; Animations Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -880,13 +1026,15 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning CSS UI Toolkits Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -896,13 +1044,15 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Web Development Data APIs Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -912,13 +1062,15 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Desktop Application Development with Web Technologies Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -928,13 +1080,15 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning DOM, BOM, &amp; CSSOM Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -944,13 +1098,15 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning The Front End Developer Profession Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -960,13 +1116,15 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Front End Development Technology Overview Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -976,13 +1134,15 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Getting a Front End Developer Job Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -992,13 +1152,15 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Git Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -1008,13 +1170,15 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning HTML Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
@@ -1024,13 +1188,15 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning HTML Email Development Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -1040,13 +1206,15 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning HTTP Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -1056,13 +1224,15 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JAM Stack Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
@@ -1072,13 +1242,15 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Fundamentals Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
@@ -1088,13 +1260,15 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Modules &amp; Scripts Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
@@ -1104,13 +1278,15 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Regular Expressions Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
@@ -1120,13 +1296,15 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Animation Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
@@ -1136,13 +1314,15 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Application Frameworks/Libraries Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
@@ -1152,13 +1332,15 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Asynchronous Programming Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
@@ -1168,13 +1350,15 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Bundlers Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
@@ -1184,13 +1368,15 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Compile to JS Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
@@ -1200,13 +1386,15 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript &amp; Computer Science Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
@@ -1216,13 +1404,15 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="D35" s="3"/>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Functional Programming (FP) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
@@ -1232,13 +1422,15 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Object-Oriented Programming (OOP) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
@@ -1248,13 +1440,15 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
@@ -1264,13 +1458,15 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="D38" s="3"/>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Practices &amp; Tooling Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="1"/>
@@ -1280,13 +1476,15 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Runtime &amp; AST Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="1"/>
@@ -1296,13 +1494,15 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript State Management Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="1"/>
@@ -1312,13 +1512,15 @@
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="D41" s="3"/>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript UI Components and Widgets Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="1"/>
@@ -1328,13 +1530,15 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="D42" s="3"/>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Web APIs Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="1"/>
@@ -1344,13 +1548,15 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Native Mobile Applications Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="1"/>
@@ -1360,13 +1566,15 @@
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Node.js &amp; npm / Yarn Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="1"/>
@@ -1376,13 +1584,15 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning npm &amp; yarn Scripts Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="1"/>
@@ -1392,13 +1602,15 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Progressive Web Apps (PWAs) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="1"/>
@@ -1408,13 +1620,15 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="D47" s="3"/>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Responsive Web Design Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="1"/>
@@ -1424,13 +1638,15 @@
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D48" s="3"/>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Search Engine Optimization (SEO) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="1"/>
@@ -1440,13 +1656,15 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="D49" s="3"/>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Unit and End-to-End Testing Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="1"/>
@@ -1456,13 +1674,15 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning The Web Platform Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="1"/>
@@ -1471,14 +1691,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
-      <c r="B51" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51" s="3"/>
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="D51" s="3"/>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning UI Design / Patterns Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="1"/>
@@ -1487,14 +1709,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
-      <c r="B52" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="3"/>
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="D52" s="3"/>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Web Applications Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="1"/>
@@ -1503,14 +1727,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
-      <c r="B53" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" s="3"/>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="D53" s="3"/>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Web Images Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="1"/>
@@ -1519,14 +1745,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
-      <c r="B54" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="3"/>
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="D54" s="3"/>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Web Security Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="1"/>
@@ -1535,14 +1763,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
-      <c r="B55" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="3"/>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="D55" s="3"/>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Web Developer Tools Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="1"/>
@@ -1551,14 +1781,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
-      <c r="B56" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="3"/>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="D56" s="3"/>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning World Wide Web (WWW) Basic Mechanics Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="1"/>
@@ -1567,14 +1799,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
-      <c r="B57" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="3"/>
+      <c r="B57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="D57" s="3"/>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning Compile to JavaScript Languages Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="1"/>
@@ -1583,9 +1817,6 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
-      <c r="B58" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" t="str">
@@ -1599,9 +1830,6 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
-      <c r="B59" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" t="str">

</xml_diff>

<commit_message>
Update Beta tag markup, update guide links
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/projects/learning-roadmap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/Projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24561962-BC5B-F146-9BD4-3FC259607876}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BA000F-63F1-B643-B917-D4275A1277B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
+    <workbookView xWindow="46960" yWindow="-4620" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,9 +339,6 @@
     <t>JavaScript UI Components and Widgets</t>
   </si>
   <si>
-    <t>JavaScript Web APIs</t>
-  </si>
-  <si>
     <t>Native Mobile Applications</t>
   </si>
   <si>
@@ -388,6 +385,9 @@
   </si>
   <si>
     <t>World Wide Web (WWW) Basic Mechanics</t>
+  </si>
+  <si>
+    <t>JavaScript Web Platform APIs</t>
   </si>
 </sst>
 </file>
@@ -775,7 +775,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1116,7 +1116,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>78</v>
@@ -1533,12 +1533,12 @@
         <v>37</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Web APIs Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Learning JavaScript Web Platform APIs Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="1"/>
@@ -1551,7 +1551,7 @@
         <v>38</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="str">
@@ -1569,7 +1569,7 @@
         <v>39</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" t="str">
@@ -1587,7 +1587,7 @@
         <v>40</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" t="str">
@@ -1605,7 +1605,7 @@
         <v>41</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" t="str">
@@ -1623,7 +1623,7 @@
         <v>42</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" t="str">
@@ -1641,7 +1641,7 @@
         <v>43</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" t="str">
@@ -1659,7 +1659,7 @@
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" t="str">
@@ -1677,7 +1677,7 @@
         <v>45</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" t="str">
@@ -1695,7 +1695,7 @@
         <v>46</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" t="str">
@@ -1713,7 +1713,7 @@
         <v>47</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" t="str">
@@ -1731,7 +1731,7 @@
         <v>48</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" t="str">
@@ -1749,7 +1749,7 @@
         <v>49</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" t="str">
@@ -1767,7 +1767,7 @@
         <v>50</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" t="str">
@@ -1785,7 +1785,7 @@
         <v>71</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" t="str">
@@ -1803,7 +1803,7 @@
         <v>51</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" t="str">

</xml_diff>

<commit_message>
Start updating SEO-friendly titles
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/Projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BA000F-63F1-B643-B917-D4275A1277B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D88F4D8-C2E6-AE4A-9BAC-987239FE191B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46960" yWindow="-4620" windowWidth="28040" windowHeight="17440" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
+    <workbookView xWindow="38540" yWindow="-4620" windowWidth="46520" windowHeight="19100" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>CSS Fundamentals</t>
   </si>
   <si>
-    <t>CSS in JavaScript</t>
-  </si>
-  <si>
     <t>CSS Layout</t>
   </si>
   <si>
@@ -388,13 +385,16 @@
   </si>
   <si>
     <t>JavaScript Web Platform APIs</t>
+  </si>
+  <si>
+    <t>CSS in JavaScript (CSS-in-JS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,6 +420,12 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -452,11 +458,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -774,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051CB134-E970-F24C-8599-A156C71AD5D0}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,8 +824,8 @@
         <v>57</v>
       </c>
       <c r="E2" t="str">
-        <f>"&lt;title&gt;Learning "&amp;C2&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Web Accessibility Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <f>"&lt;title&gt;"&amp;C2&amp;" Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
+        <v>&lt;title&gt;Web Accessibility Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F2" t="str">
         <f>"&lt;meta name='description' content=''"&amp;D2&amp;"'&gt;"</f>
@@ -835,8 +842,8 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E59" si="0">"&lt;title&gt;Learning "&amp;C3&amp;" Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
-        <v>&lt;title&gt;Learning Browser, Website, and Web App Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <f t="shared" ref="E3:E59" si="0">"&lt;title&gt;"&amp;C3&amp;" Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;"</f>
+        <v>&lt;title&gt;Browser, Website, and Web App Performance Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F59" si="1">"&lt;meta name='description' content=''"&amp;D3&amp;"'&gt;"</f>
@@ -854,7 +861,7 @@
       <c r="D4" s="3"/>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Code Editors Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Code Editors Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -872,7 +879,7 @@
       <c r="D5" s="3"/>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Command Line Interface Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Command Line Interface Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -890,7 +897,7 @@
       <c r="D6" s="3"/>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Fonts &amp; Icons Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Fonts &amp; Icons Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -908,7 +915,7 @@
       <c r="D7" s="3"/>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Fundamentals Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Fundamentals Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -920,13 +927,13 @@
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>64</v>
+      <c r="C8" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS in JavaScript Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS in JavaScript (CSS-in-JS) Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -939,12 +946,12 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Layout Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Layout Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -957,12 +964,12 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Media Queries Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Media Queries Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -975,12 +982,12 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Best Practices Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Best Practices Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -993,12 +1000,12 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Tooling Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Tooling Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -1008,15 +1015,15 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS Transitions, Transforms, &amp; Animations Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS Transitions, Transforms, &amp; Animations Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -1029,12 +1036,12 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning CSS UI Toolkits Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;CSS UI Toolkits Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -1047,12 +1054,12 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Web Development Data APIs Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Web Development Data APIs Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -1065,12 +1072,12 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Desktop Application Development with Web Technologies Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Desktop Application Development with Web Technologies Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -1083,12 +1090,12 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning DOM, BOM, &amp; CSSOM Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;DOM, BOM, &amp; CSSOM Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -1098,15 +1105,15 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning The Front End Developer Profession Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;The Front End Developer Profession Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -1116,15 +1123,15 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Front End Development Technology Overview Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Front End Development Technology Overview Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -1137,12 +1144,12 @@
         <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Getting a Front End Developer Job Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Getting a Front End Developer Job Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -1155,12 +1162,12 @@
         <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Git Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Git Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -1173,12 +1180,12 @@
         <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning HTML Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;HTML Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
@@ -1191,12 +1198,12 @@
         <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning HTML Email Development Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;HTML Email Development Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -1209,12 +1216,12 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning HTTP Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;HTTP Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -1227,12 +1234,12 @@
         <v>20</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JAM Stack Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JAM Stack Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
@@ -1245,12 +1252,12 @@
         <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Fundamentals Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Fundamentals Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
@@ -1263,12 +1270,12 @@
         <v>22</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Modules &amp; Scripts Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Modules &amp; Scripts Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
@@ -1281,12 +1288,12 @@
         <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Regular Expressions Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Regular Expressions Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
@@ -1299,12 +1306,12 @@
         <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Animation Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Animation Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
@@ -1317,12 +1324,12 @@
         <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Application Frameworks/Libraries Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Application Frameworks/Libraries Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
@@ -1335,12 +1342,12 @@
         <v>26</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Asynchronous Programming Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Asynchronous Programming Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
@@ -1353,12 +1360,12 @@
         <v>27</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Bundlers Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Bundlers Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
@@ -1371,12 +1378,12 @@
         <v>28</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Compile to JS Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Compile to JS Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
@@ -1389,12 +1396,12 @@
         <v>29</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript &amp; Computer Science Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript &amp; Computer Science Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
@@ -1407,12 +1414,12 @@
         <v>30</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Functional Programming (FP) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Functional Programming (FP) Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
@@ -1425,12 +1432,12 @@
         <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Object-Oriented Programming (OOP) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Object-Oriented Programming (OOP) Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
@@ -1443,12 +1450,12 @@
         <v>32</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Performance Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Performance Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
@@ -1461,12 +1468,12 @@
         <v>33</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Practices &amp; Tooling Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Practices &amp; Tooling Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="1"/>
@@ -1479,12 +1486,12 @@
         <v>34</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Runtime &amp; AST Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Runtime &amp; AST Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="1"/>
@@ -1497,12 +1504,12 @@
         <v>35</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript State Management Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript State Management Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="1"/>
@@ -1515,12 +1522,12 @@
         <v>36</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript UI Components and Widgets Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript UI Components and Widgets Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="1"/>
@@ -1533,12 +1540,12 @@
         <v>37</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Web Platform APIs Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Web Platform APIs Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="1"/>
@@ -1551,12 +1558,12 @@
         <v>38</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Native Mobile Applications Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Native Mobile Applications Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="1"/>
@@ -1569,12 +1576,12 @@
         <v>39</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Node.js &amp; npm / Yarn Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Node.js &amp; npm / Yarn Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="1"/>
@@ -1587,12 +1594,12 @@
         <v>40</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning npm &amp; yarn Scripts Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;npm &amp; yarn Scripts Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="1"/>
@@ -1605,12 +1612,12 @@
         <v>41</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Progressive Web Apps (PWAs) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Progressive Web Apps (PWAs) Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="1"/>
@@ -1623,12 +1630,12 @@
         <v>42</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Responsive Web Design Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Responsive Web Design Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="1"/>
@@ -1641,12 +1648,12 @@
         <v>43</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Search Engine Optimization (SEO) Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Search Engine Optimization (SEO) Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="1"/>
@@ -1659,12 +1666,12 @@
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning JavaScript Unit and End-to-End Testing Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;JavaScript Unit and End-to-End Testing Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="1"/>
@@ -1677,12 +1684,12 @@
         <v>45</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning The Web Platform Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;The Web Platform Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="1"/>
@@ -1695,12 +1702,12 @@
         <v>46</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning UI Design / Patterns Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;UI Design / Patterns Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="1"/>
@@ -1713,12 +1720,12 @@
         <v>47</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Web Applications Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Web Applications Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="1"/>
@@ -1731,12 +1738,12 @@
         <v>48</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Web Images Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Web Images Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="1"/>
@@ -1749,12 +1756,12 @@
         <v>49</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Web Security Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Web Security Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="1"/>
@@ -1767,12 +1774,12 @@
         <v>50</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Web Developer Tools Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Web Developer Tools Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="1"/>
@@ -1782,15 +1789,15 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning World Wide Web (WWW) Basic Mechanics Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;World Wide Web (WWW) Basic Mechanics Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="1"/>
@@ -1803,12 +1810,12 @@
         <v>51</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning Compile to JavaScript Languages Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt;Compile to JavaScript Languages Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="1"/>
@@ -1821,7 +1828,7 @@
       <c r="D58" s="3"/>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt; Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="1"/>
@@ -1834,7 +1841,7 @@
       <c r="D59" s="3"/>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;title&gt;Learning  Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
+        <v>&lt;title&gt; Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Add generated table of contents
</commit_message>
<xml_diff>
--- a/meta.xlsx
+++ b/meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcgrabanski/Sites/Projects/learning-roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D88F4D8-C2E6-AE4A-9BAC-987239FE191B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A4D8B9-90FE-A144-B945-FB3F17DB0436}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38540" yWindow="-4620" windowWidth="46520" windowHeight="19100" xr2:uid="{96C34D49-0A4B-B343-8DE8-41C74F167C28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>accessibility</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>CSS in JavaScript (CSS-in-JS)</t>
+  </si>
+  <si>
+    <t>Generated TOC</t>
   </si>
 </sst>
 </file>
@@ -779,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051CB134-E970-F24C-8599-A156C71AD5D0}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,11 +793,11 @@
     <col min="2" max="2" width="36.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" customWidth="1"/>
     <col min="4" max="4" width="65.6640625" customWidth="1"/>
-    <col min="5" max="5" width="104.83203125" customWidth="1"/>
-    <col min="6" max="6" width="85.5" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>53</v>
@@ -811,8 +814,11 @@
       <c r="F1" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -831,8 +837,12 @@
         <f>"&lt;meta name='description' content=''"&amp;D2&amp;"'&gt;"</f>
         <v>&lt;meta name='description' content=''Learning resources for eb accessibility means that everyone, including people with disabilities, can use your Websites.'&gt;</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="str">
+        <f>"&lt;li&gt;&lt;a href='"&amp;B2&amp;"/' target='_blank'&gt;"&amp;C2&amp;" Learning Resources&lt;/a&gt;&lt;/li&gt;"</f>
+        <v>&lt;li&gt;&lt;a href='accessibility/' target='_blank'&gt;Web Accessibility Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -849,8 +859,12 @@
         <f t="shared" ref="F3:F59" si="1">"&lt;meta name='description' content=''"&amp;D3&amp;"'&gt;"</f>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G57" si="2">"&lt;li&gt;&lt;a href='"&amp;B3&amp;"/' target='_blank'&gt;"&amp;C3&amp;" Learning Resources&lt;/a&gt;&lt;/li&gt;"</f>
+        <v>&lt;li&gt;&lt;a href='browser-webpage-performance/' target='_blank'&gt;Browser, Website, and Web App Performance Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>2</v>
@@ -867,8 +881,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='code-editors/' target='_blank'&gt;Code Editors Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>3</v>
@@ -885,8 +903,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='command-line-interface/' target='_blank'&gt;Command Line Interface Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -903,8 +925,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-fonts-and-icons/' target='_blank'&gt;CSS Fonts &amp; Icons Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -921,8 +947,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-fundamentals/' target='_blank'&gt;CSS Fundamentals Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -939,8 +969,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-in-js/' target='_blank'&gt;CSS in JavaScript (CSS-in-JS) Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -957,8 +991,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-layout/' target='_blank'&gt;CSS Layout Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -975,8 +1013,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-media-queries/' target='_blank'&gt;CSS Media Queries Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -993,8 +1035,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-practices/' target='_blank'&gt;CSS Best Practices Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -1011,8 +1057,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-tooling/' target='_blank'&gt;CSS Tooling Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>68</v>
@@ -1029,8 +1079,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-transitions-transforms-animations/' target='_blank'&gt;CSS Transitions, Transforms, &amp; Animations Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -1047,8 +1101,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='css-ui-toolkits/' target='_blank'&gt;CSS UI Toolkits Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -1065,8 +1123,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='data-apis/' target='_blank'&gt;Web Development Data APIs Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>13</v>
@@ -1083,8 +1145,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='desktop-apps/' target='_blank'&gt;Desktop Application Development with Web Technologies Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>14</v>
@@ -1101,8 +1167,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='dom-bom-cssom/' target='_blank'&gt;DOM, BOM, &amp; CSSOM Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>69</v>
@@ -1119,8 +1189,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='front-end-developer-profession/' target='_blank'&gt;The Front End Developer Profession Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>113</v>
@@ -1137,8 +1211,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='front-end-development-overview/' target='_blank'&gt;Front End Development Technology Overview Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>15</v>
@@ -1155,8 +1233,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='getting-a-front-end-developer-job/' target='_blank'&gt;Getting a Front End Developer Job Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>16</v>
@@ -1173,8 +1255,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='git/' target='_blank'&gt;Git Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>17</v>
@@ -1191,8 +1277,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='html/' target='_blank'&gt;HTML Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>18</v>
@@ -1209,8 +1299,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='html-email/' target='_blank'&gt;HTML Email Development Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>19</v>
@@ -1227,8 +1321,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='http/' target='_blank'&gt;HTTP Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>20</v>
@@ -1245,8 +1343,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='jam-stack/' target='_blank'&gt;JAM Stack Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>21</v>
@@ -1263,8 +1365,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='javascript-fundamentals/' target='_blank'&gt;JavaScript Fundamentals Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>22</v>
@@ -1281,8 +1387,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='javascript-modules-scripts/' target='_blank'&gt;JavaScript Modules &amp; Scripts Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>23</v>
@@ -1299,8 +1409,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='javascript-regular-expressions/' target='_blank'&gt;JavaScript Regular Expressions Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
         <v>24</v>
@@ -1317,8 +1431,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-animation/' target='_blank'&gt;JavaScript Animation Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>25</v>
@@ -1335,8 +1453,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-app-frameworks/' target='_blank'&gt;JavaScript Application Frameworks/Libraries Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
         <v>26</v>
@@ -1353,8 +1475,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-async/' target='_blank'&gt;JavaScript Asynchronous Programming Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
         <v>27</v>
@@ -1371,8 +1497,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-bundlers/' target='_blank'&gt;JavaScript Bundlers Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>28</v>
@@ -1389,8 +1519,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-compile-to-js/' target='_blank'&gt;JavaScript Compile to JS Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>29</v>
@@ -1407,8 +1541,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-cs/' target='_blank'&gt;JavaScript &amp; Computer Science Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
         <v>30</v>
@@ -1425,8 +1563,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-fp/' target='_blank'&gt;JavaScript Functional Programming (FP) Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>31</v>
@@ -1443,8 +1585,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-oop/' target='_blank'&gt;JavaScript Object-Oriented Programming (OOP) Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
         <v>32</v>
@@ -1461,8 +1607,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-performance/' target='_blank'&gt;JavaScript Performance Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>33</v>
@@ -1479,8 +1629,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-practices-tools/' target='_blank'&gt;JavaScript Practices &amp; Tooling Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
         <v>34</v>
@@ -1497,8 +1651,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-runtime-ast/' target='_blank'&gt;JavaScript Runtime &amp; AST Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>35</v>
@@ -1515,8 +1673,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-state-management/' target='_blank'&gt;JavaScript State Management Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
         <v>36</v>
@@ -1533,8 +1695,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-ui-components-and-widgets/' target='_blank'&gt;JavaScript UI Components and Widgets Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>37</v>
@@ -1551,8 +1717,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='js-web-api/' target='_blank'&gt;JavaScript Web Platform APIs Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
         <v>38</v>
@@ -1569,8 +1739,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='mobile-apps/' target='_blank'&gt;Native Mobile Applications Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>39</v>
@@ -1587,8 +1761,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='node-npm/' target='_blank'&gt;Node.js &amp; npm / Yarn Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>40</v>
@@ -1605,8 +1783,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='npm-yarn-scripts/' target='_blank'&gt;npm &amp; yarn Scripts Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
         <v>41</v>
@@ -1623,8 +1805,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='pwa/' target='_blank'&gt;Progressive Web Apps (PWAs) Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>42</v>
@@ -1641,8 +1827,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='rwd/' target='_blank'&gt;Responsive Web Design Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>43</v>
@@ -1659,8 +1849,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='seo/' target='_blank'&gt;Search Engine Optimization (SEO) Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>44</v>
@@ -1677,8 +1871,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='testing/' target='_blank'&gt;JavaScript Unit and End-to-End Testing Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
         <v>45</v>
@@ -1695,8 +1893,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='the-web-platform/' target='_blank'&gt;The Web Platform Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" t="s">
         <v>46</v>
@@ -1713,8 +1915,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='ui-design-patterns/' target='_blank'&gt;UI Design / Patterns Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" t="s">
         <v>47</v>
@@ -1731,8 +1937,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='web-apps/' target='_blank'&gt;Web Applications Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" t="s">
         <v>48</v>
@@ -1749,8 +1959,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='web-images/' target='_blank'&gt;Web Images Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" t="s">
         <v>49</v>
@@ -1767,8 +1981,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='web-security/' target='_blank'&gt;Web Security Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" t="s">
         <v>50</v>
@@ -1785,8 +2003,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='webdev-tools/' target='_blank'&gt;Web Developer Tools Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" t="s">
         <v>70</v>
@@ -1803,8 +2025,12 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='www-basic-mechanics/' target='_blank'&gt;World Wide Web (WWW) Basic Mechanics Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" t="s">
         <v>51</v>
@@ -1821,32 +2047,20 @@
         <f t="shared" si="1"/>
         <v>&lt;meta name='description' content='''&gt;</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;li&gt;&lt;a href='x-compile-to-js/' target='_blank'&gt;Compile to JavaScript Languages Learning Resources&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
-      <c r="E58" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;title&gt; Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-      <c r="F58" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta name='description' content='''&gt;</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
-      <c r="E59" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;title&gt; Learning Resources - Front-End Developer Learning Roadmap&lt;/title&gt;</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;meta name='description' content='''&gt;</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>